<commit_message>
Added week 5 work
</commit_message>
<xml_diff>
--- a/FYP Gantt Chart.xlsx
+++ b/FYP Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6700845d1be91df/Documents/FYP 2023/week2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FYP notes\FYP 2023\week5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_F25DC773A252ABDACC104874091965705ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD1E8682-E419-440A-9947-20DD8FCB0775}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF20067F-D99F-46DF-BD85-88AFF7D91D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,6 @@
     <t>Days to Complete</t>
   </si>
   <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
     <t>Task 5</t>
   </si>
   <si>
@@ -79,6 +67,18 @@
   </si>
   <si>
     <t>Task 15</t>
+  </si>
+  <si>
+    <t>Draft Report</t>
+  </si>
+  <si>
+    <t>Repair Flow Chart</t>
+  </si>
+  <si>
+    <t>Repair Research</t>
+  </si>
+  <si>
+    <t>Article Research</t>
   </si>
 </sst>
 </file>
@@ -224,16 +224,16 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Task 1</c:v>
+                  <c:v>Repair Research</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Task 2</c:v>
+                  <c:v>Draft Report</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Task 3</c:v>
+                  <c:v>Repair Flow Chart</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Task 4</c:v>
+                  <c:v>Article Research</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Task 5</c:v>
@@ -326,16 +326,16 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Task 1</c:v>
+                  <c:v>Repair Research</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Task 2</c:v>
+                  <c:v>Draft Report</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Task 3</c:v>
+                  <c:v>Repair Flow Chart</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Task 4</c:v>
+                  <c:v>Article Research</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Task 5</c:v>
@@ -1406,11 +1406,12 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1428,7 +1429,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>45174</v>
@@ -1439,7 +1440,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>45193</v>
@@ -1450,7 +1451,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>45180</v>
@@ -1461,62 +1462,62 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added week 6 work
</commit_message>
<xml_diff>
--- a/FYP Gantt Chart.xlsx
+++ b/FYP Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FYP notes\FYP 2023\week5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP notes\FYP 2023\week6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF20067F-D99F-46DF-BD85-88AFF7D91D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965DADA8-7CA5-425E-9629-4E288EF8B1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Days to Complete</t>
   </si>
   <si>
-    <t>Task 5</t>
-  </si>
-  <si>
     <t>Task 6</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Article Research</t>
+  </si>
+  <si>
+    <t>Task Automating Identification</t>
   </si>
 </sst>
 </file>
@@ -236,7 +236,7 @@
                   <c:v>Article Research</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 5</c:v>
+                  <c:v>Task Automating Identification</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Task 6</c:v>
@@ -285,6 +285,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,7 +344,7 @@
                   <c:v>Article Research</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 5</c:v>
+                  <c:v>Task Automating Identification</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Task 6</c:v>
@@ -386,7 +392,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -516,7 +528,11 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1104,15 +1120,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>40005</xdr:colOff>
+      <xdr:colOff>40004</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>188595</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>257735</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1406,17 +1422,17 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1427,9 +1443,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>45174</v>
@@ -1438,9 +1454,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>45193</v>
@@ -1449,81 +1465,91 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>45180</v>
       </c>
       <c r="C4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45186</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45185</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
-        <v>45174</v>
-      </c>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added week 14 work
</commit_message>
<xml_diff>
--- a/FYP Gantt Chart.xlsx
+++ b/FYP Gantt Chart.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP notes\FYP 2023\week6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FYP notes\FYP 2023\week14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965DADA8-7CA5-425E-9629-4E288EF8B1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20908CD0-C8C8-47A7-8E96-EFFD049FB292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +37,6 @@
     <t>Days to Complete</t>
   </si>
   <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>Task 7</t>
-  </si>
-  <si>
     <t>Task 8</t>
   </si>
   <si>
@@ -79,6 +74,12 @@
   </si>
   <si>
     <t>Task Automating Identification</t>
+  </si>
+  <si>
+    <t>Uni Break</t>
+  </si>
+  <si>
+    <t>Prototype Research</t>
   </si>
 </sst>
 </file>
@@ -239,10 +240,10 @@
                   <c:v>Task Automating Identification</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Task 6</c:v>
+                  <c:v>Uni Break</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Task 7</c:v>
+                  <c:v>Prototype Research</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Task 8</c:v>
@@ -291,6 +292,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45185</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45249</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,10 +354,10 @@
                   <c:v>Task Automating Identification</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Task 6</c:v>
+                  <c:v>Uni Break</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Task 7</c:v>
+                  <c:v>Prototype Research</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Task 8</c:v>
@@ -395,10 +402,16 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1422,7 +1435,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,7 +1458,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>45174</v>
@@ -1456,7 +1469,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>45193</v>
@@ -1467,7 +1480,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>45180</v>
@@ -1478,18 +1491,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>45186</v>
       </c>
       <c r="C5">
-        <v>64</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>45185</v>
@@ -1500,52 +1513,64 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45249</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45343</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added week 15 work
</commit_message>
<xml_diff>
--- a/FYP Gantt Chart.xlsx
+++ b/FYP Gantt Chart.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FYP notes\FYP 2023\week14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP notes\FYP 2023\week15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20908CD0-C8C8-47A7-8E96-EFFD049FB292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF88451C-FD85-4BE7-B7A8-6492DFBEEC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
Added week 16 work
</commit_message>
<xml_diff>
--- a/FYP Gantt Chart.xlsx
+++ b/FYP Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP notes\FYP 2023\week15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FYP notes\FYP 2023\week16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF88451C-FD85-4BE7-B7A8-6492DFBEEC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB907EAC-8A21-45AF-B4E1-48165A71A895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,6 @@
     <t>Days to Complete</t>
   </si>
   <si>
-    <t>Task 8</t>
-  </si>
-  <si>
-    <t>Task 9</t>
-  </si>
-  <si>
     <t>Task 10</t>
   </si>
   <si>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>Prototype Research</t>
+  </si>
+  <si>
+    <t>Modelling</t>
+  </si>
+  <si>
+    <t>Prototype 3D Model</t>
   </si>
 </sst>
 </file>
@@ -245,10 +245,10 @@
                   <c:v>Prototype Research</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Task 8</c:v>
+                  <c:v>Modelling</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Task 9</c:v>
+                  <c:v>Prototype 3D Model</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Task 10</c:v>
@@ -297,6 +297,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45398</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45390</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,10 +365,10 @@
                   <c:v>Prototype Research</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Task 8</c:v>
+                  <c:v>Modelling</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Task 9</c:v>
+                  <c:v>Prototype 3D Model</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Task 10</c:v>
@@ -411,6 +417,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1434,17 +1446,17 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1455,9 +1467,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>45174</v>
@@ -1466,9 +1478,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>45193</v>
@@ -1477,9 +1489,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>45180</v>
@@ -1488,9 +1500,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>45186</v>
@@ -1499,9 +1511,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>45185</v>
@@ -1510,9 +1522,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>45249</v>
@@ -1521,9 +1533,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>45343</v>
@@ -1532,47 +1544,59 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45398</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45390</v>
+      </c>
+      <c r="C10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
     </row>
   </sheetData>

</xml_diff>